<commit_message>
Riak dotestování s konfigurací případné konzistence
</commit_message>
<xml_diff>
--- a/Tests/KDBS_Vysledky_testu.xlsx
+++ b/Tests/KDBS_Vysledky_testu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HDD_VSB\Git VŠB - StandAlones\DP-KVDBS\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DFCC48D-2F1E-47F3-82AC-E94EA0EA3BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C24869D-70FE-49E9-8BBA-18716BE94913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Workloads - Read, Update" sheetId="1" r:id="rId1"/>
@@ -10943,7 +10943,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
@@ -12050,8 +12050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E628E191-458C-48C1-BA88-DA60FE101777}">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>